<commit_message>
Attempt to add 7th
Didn't work, had to revert because filter wasn't formatting how I wanted.
</commit_message>
<xml_diff>
--- a/Chord_Chart_Source.xlsx
+++ b/Chord_Chart_Source.xlsx
@@ -9,12 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15480" windowHeight="7455"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15480" windowHeight="7455" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Basic Notes" sheetId="1" r:id="rId1"/>
     <sheet name="Chords" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Chords!$A$1:$G$43</definedName>
+  </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -25,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="44">
   <si>
     <t>Note</t>
   </si>
@@ -151,6 +154,12 @@
   </si>
   <si>
     <t>1B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>7th</t>
   </si>
 </sst>
 </file>
@@ -186,8 +195,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -470,7 +480,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
@@ -774,8 +784,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:XFD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -790,8 +800,8 @@
       <c r="B1" t="s">
         <v>5</v>
       </c>
-      <c r="C1">
-        <v>7</v>
+      <c r="C1" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="D1" t="s">
         <v>6</v>
@@ -808,13 +818,22 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
       </c>
+      <c r="C2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E2" t="s">
+        <v>42</v>
+      </c>
       <c r="F2" t="s">
-        <v>17</v>
+        <v>39</v>
       </c>
       <c r="G2">
         <v>1</v>
@@ -822,13 +841,22 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>
       </c>
+      <c r="C3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E3" t="s">
+        <v>42</v>
+      </c>
       <c r="F3" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="G3">
         <v>3</v>
@@ -836,13 +864,22 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
       </c>
+      <c r="C4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E4" t="s">
+        <v>42</v>
+      </c>
       <c r="F4" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="G4">
         <v>5</v>
@@ -850,13 +887,22 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
       </c>
+      <c r="C5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E5" t="s">
+        <v>42</v>
+      </c>
       <c r="F5" t="s">
-        <v>17</v>
+        <v>39</v>
       </c>
       <c r="G5">
         <v>1</v>
@@ -864,13 +910,22 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
       </c>
+      <c r="C6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E6" t="s">
+        <v>42</v>
+      </c>
       <c r="F6" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="G6">
         <v>3</v>
@@ -878,13 +933,22 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B7" t="s">
         <v>10</v>
       </c>
+      <c r="C7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7" t="s">
+        <v>42</v>
+      </c>
+      <c r="E7" t="s">
+        <v>42</v>
+      </c>
       <c r="F7" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="G7">
         <v>5</v>
@@ -892,13 +956,22 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B8" t="s">
         <v>8</v>
       </c>
+      <c r="C8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D8" t="s">
+        <v>42</v>
+      </c>
+      <c r="E8" t="s">
+        <v>42</v>
+      </c>
       <c r="F8" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G8">
         <v>1</v>
@@ -906,13 +979,22 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B9" t="s">
         <v>8</v>
       </c>
+      <c r="C9" t="s">
+        <v>42</v>
+      </c>
+      <c r="D9" t="s">
+        <v>42</v>
+      </c>
+      <c r="E9" t="s">
+        <v>42</v>
+      </c>
       <c r="F9" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G9">
         <v>3</v>
@@ -920,13 +1002,22 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B10" t="s">
         <v>8</v>
       </c>
+      <c r="C10" t="s">
+        <v>42</v>
+      </c>
+      <c r="D10" t="s">
+        <v>42</v>
+      </c>
+      <c r="E10" t="s">
+        <v>42</v>
+      </c>
       <c r="F10" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="G10">
         <v>5</v>
@@ -934,13 +1025,22 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B11" t="s">
         <v>10</v>
       </c>
+      <c r="C11" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" t="s">
+        <v>42</v>
+      </c>
+      <c r="E11" t="s">
+        <v>42</v>
+      </c>
       <c r="F11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G11">
         <v>1</v>
@@ -948,13 +1048,22 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B12" t="s">
         <v>10</v>
       </c>
+      <c r="C12" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" t="s">
+        <v>42</v>
+      </c>
+      <c r="E12" t="s">
+        <v>42</v>
+      </c>
       <c r="F12" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G12">
         <v>3</v>
@@ -962,13 +1071,22 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B13" t="s">
         <v>10</v>
       </c>
+      <c r="C13" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" t="s">
+        <v>42</v>
+      </c>
+      <c r="E13" t="s">
+        <v>42</v>
+      </c>
       <c r="F13" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="G13">
         <v>5</v>
@@ -976,13 +1094,22 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="B14" t="s">
         <v>8</v>
       </c>
+      <c r="C14" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" t="s">
+        <v>42</v>
+      </c>
+      <c r="E14" t="s">
+        <v>42</v>
+      </c>
       <c r="F14" t="s">
-        <v>41</v>
+        <v>17</v>
       </c>
       <c r="G14">
         <v>1</v>
@@ -990,13 +1117,22 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="B15" t="s">
         <v>8</v>
       </c>
+      <c r="C15" t="s">
+        <v>42</v>
+      </c>
+      <c r="D15" t="s">
+        <v>42</v>
+      </c>
+      <c r="E15" t="s">
+        <v>42</v>
+      </c>
       <c r="F15" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="G15">
         <v>3</v>
@@ -1004,13 +1140,22 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="B16" t="s">
         <v>8</v>
       </c>
+      <c r="C16" t="s">
+        <v>42</v>
+      </c>
+      <c r="D16" t="s">
+        <v>42</v>
+      </c>
+      <c r="E16" t="s">
+        <v>42</v>
+      </c>
       <c r="F16" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="G16">
         <v>5</v>
@@ -1018,13 +1163,22 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="B17" t="s">
         <v>10</v>
       </c>
+      <c r="C17" t="s">
+        <v>42</v>
+      </c>
+      <c r="D17" t="s">
+        <v>42</v>
+      </c>
+      <c r="E17" t="s">
+        <v>42</v>
+      </c>
       <c r="F17" t="s">
-        <v>41</v>
+        <v>17</v>
       </c>
       <c r="G17">
         <v>1</v>
@@ -1032,13 +1186,22 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="B18" t="s">
         <v>10</v>
       </c>
+      <c r="C18" t="s">
+        <v>42</v>
+      </c>
+      <c r="D18" t="s">
+        <v>42</v>
+      </c>
+      <c r="E18" t="s">
+        <v>42</v>
+      </c>
       <c r="F18" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="G18">
         <v>3</v>
@@ -1046,13 +1209,22 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="B19" t="s">
         <v>10</v>
       </c>
+      <c r="C19" t="s">
+        <v>42</v>
+      </c>
+      <c r="D19" t="s">
+        <v>42</v>
+      </c>
+      <c r="E19" t="s">
+        <v>42</v>
+      </c>
       <c r="F19" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="G19">
         <v>5</v>
@@ -1065,6 +1237,15 @@
       <c r="B20" t="s">
         <v>8</v>
       </c>
+      <c r="C20" t="s">
+        <v>42</v>
+      </c>
+      <c r="D20" t="s">
+        <v>42</v>
+      </c>
+      <c r="E20" t="s">
+        <v>42</v>
+      </c>
       <c r="F20" t="s">
         <v>18</v>
       </c>
@@ -1079,6 +1260,15 @@
       <c r="B21" t="s">
         <v>8</v>
       </c>
+      <c r="C21" t="s">
+        <v>42</v>
+      </c>
+      <c r="D21" t="s">
+        <v>42</v>
+      </c>
+      <c r="E21" t="s">
+        <v>42</v>
+      </c>
       <c r="F21" t="s">
         <v>32</v>
       </c>
@@ -1093,6 +1283,15 @@
       <c r="B22" t="s">
         <v>8</v>
       </c>
+      <c r="C22" t="s">
+        <v>42</v>
+      </c>
+      <c r="D22" t="s">
+        <v>42</v>
+      </c>
+      <c r="E22" t="s">
+        <v>42</v>
+      </c>
       <c r="F22" t="s">
         <v>39</v>
       </c>
@@ -1107,6 +1306,15 @@
       <c r="B23" t="s">
         <v>10</v>
       </c>
+      <c r="C23" t="s">
+        <v>42</v>
+      </c>
+      <c r="D23" t="s">
+        <v>42</v>
+      </c>
+      <c r="E23" t="s">
+        <v>42</v>
+      </c>
       <c r="F23" t="s">
         <v>18</v>
       </c>
@@ -1121,6 +1329,15 @@
       <c r="B24" t="s">
         <v>10</v>
       </c>
+      <c r="C24" t="s">
+        <v>42</v>
+      </c>
+      <c r="D24" t="s">
+        <v>42</v>
+      </c>
+      <c r="E24" t="s">
+        <v>42</v>
+      </c>
       <c r="F24" t="s">
         <v>20</v>
       </c>
@@ -1135,6 +1352,15 @@
       <c r="B25" t="s">
         <v>10</v>
       </c>
+      <c r="C25" t="s">
+        <v>42</v>
+      </c>
+      <c r="D25" t="s">
+        <v>42</v>
+      </c>
+      <c r="E25" t="s">
+        <v>42</v>
+      </c>
       <c r="F25" t="s">
         <v>39</v>
       </c>
@@ -1149,6 +1375,15 @@
       <c r="B26" t="s">
         <v>8</v>
       </c>
+      <c r="C26" t="s">
+        <v>42</v>
+      </c>
+      <c r="D26" t="s">
+        <v>42</v>
+      </c>
+      <c r="E26" t="s">
+        <v>42</v>
+      </c>
       <c r="F26" t="s">
         <v>19</v>
       </c>
@@ -1163,6 +1398,15 @@
       <c r="B27" t="s">
         <v>8</v>
       </c>
+      <c r="C27" t="s">
+        <v>42</v>
+      </c>
+      <c r="D27" t="s">
+        <v>42</v>
+      </c>
+      <c r="E27" t="s">
+        <v>42</v>
+      </c>
       <c r="F27" t="s">
         <v>33</v>
       </c>
@@ -1177,6 +1421,15 @@
       <c r="B28" t="s">
         <v>8</v>
       </c>
+      <c r="C28" t="s">
+        <v>42</v>
+      </c>
+      <c r="D28" t="s">
+        <v>42</v>
+      </c>
+      <c r="E28" t="s">
+        <v>42</v>
+      </c>
       <c r="F28" t="s">
         <v>41</v>
       </c>
@@ -1191,6 +1444,15 @@
       <c r="B29" t="s">
         <v>10</v>
       </c>
+      <c r="C29" t="s">
+        <v>42</v>
+      </c>
+      <c r="D29" t="s">
+        <v>42</v>
+      </c>
+      <c r="E29" t="s">
+        <v>42</v>
+      </c>
       <c r="F29" t="s">
         <v>19</v>
       </c>
@@ -1205,6 +1467,15 @@
       <c r="B30" t="s">
         <v>10</v>
       </c>
+      <c r="C30" t="s">
+        <v>42</v>
+      </c>
+      <c r="D30" t="s">
+        <v>42</v>
+      </c>
+      <c r="E30" t="s">
+        <v>42</v>
+      </c>
       <c r="F30" t="s">
         <v>21</v>
       </c>
@@ -1219,6 +1490,15 @@
       <c r="B31" t="s">
         <v>10</v>
       </c>
+      <c r="C31" t="s">
+        <v>42</v>
+      </c>
+      <c r="D31" t="s">
+        <v>42</v>
+      </c>
+      <c r="E31" t="s">
+        <v>42</v>
+      </c>
       <c r="F31" t="s">
         <v>41</v>
       </c>
@@ -1233,6 +1513,15 @@
       <c r="B32" t="s">
         <v>8</v>
       </c>
+      <c r="C32" t="s">
+        <v>42</v>
+      </c>
+      <c r="D32" t="s">
+        <v>42</v>
+      </c>
+      <c r="E32" t="s">
+        <v>42</v>
+      </c>
       <c r="F32" t="s">
         <v>20</v>
       </c>
@@ -1247,6 +1536,15 @@
       <c r="B33" t="s">
         <v>8</v>
       </c>
+      <c r="C33" t="s">
+        <v>42</v>
+      </c>
+      <c r="D33" t="s">
+        <v>42</v>
+      </c>
+      <c r="E33" t="s">
+        <v>42</v>
+      </c>
       <c r="F33" t="s">
         <v>39</v>
       </c>
@@ -1261,6 +1559,15 @@
       <c r="B34" t="s">
         <v>8</v>
       </c>
+      <c r="C34" t="s">
+        <v>42</v>
+      </c>
+      <c r="D34" t="s">
+        <v>42</v>
+      </c>
+      <c r="E34" t="s">
+        <v>42</v>
+      </c>
       <c r="F34" t="s">
         <v>24</v>
       </c>
@@ -1275,6 +1582,15 @@
       <c r="B35" t="s">
         <v>10</v>
       </c>
+      <c r="C35" t="s">
+        <v>42</v>
+      </c>
+      <c r="D35" t="s">
+        <v>42</v>
+      </c>
+      <c r="E35" t="s">
+        <v>42</v>
+      </c>
       <c r="F35" t="s">
         <v>20</v>
       </c>
@@ -1289,6 +1605,15 @@
       <c r="B36" t="s">
         <v>10</v>
       </c>
+      <c r="C36" t="s">
+        <v>42</v>
+      </c>
+      <c r="D36" t="s">
+        <v>42</v>
+      </c>
+      <c r="E36" t="s">
+        <v>42</v>
+      </c>
       <c r="F36" t="s">
         <v>33</v>
       </c>
@@ -1303,6 +1628,15 @@
       <c r="B37" t="s">
         <v>10</v>
       </c>
+      <c r="C37" t="s">
+        <v>42</v>
+      </c>
+      <c r="D37" t="s">
+        <v>42</v>
+      </c>
+      <c r="E37" t="s">
+        <v>42</v>
+      </c>
       <c r="F37" t="s">
         <v>24</v>
       </c>
@@ -1317,6 +1651,15 @@
       <c r="B38" t="s">
         <v>8</v>
       </c>
+      <c r="C38" t="s">
+        <v>42</v>
+      </c>
+      <c r="D38" t="s">
+        <v>42</v>
+      </c>
+      <c r="E38" t="s">
+        <v>42</v>
+      </c>
       <c r="F38" t="s">
         <v>21</v>
       </c>
@@ -1331,6 +1674,15 @@
       <c r="B39" t="s">
         <v>8</v>
       </c>
+      <c r="C39" t="s">
+        <v>42</v>
+      </c>
+      <c r="D39" t="s">
+        <v>42</v>
+      </c>
+      <c r="E39" t="s">
+        <v>42</v>
+      </c>
       <c r="F39" t="s">
         <v>41</v>
       </c>
@@ -1345,6 +1697,15 @@
       <c r="B40" t="s">
         <v>8</v>
       </c>
+      <c r="C40" t="s">
+        <v>42</v>
+      </c>
+      <c r="D40" t="s">
+        <v>42</v>
+      </c>
+      <c r="E40" t="s">
+        <v>42</v>
+      </c>
       <c r="F40" t="s">
         <v>25</v>
       </c>
@@ -1359,6 +1720,15 @@
       <c r="B41" t="s">
         <v>10</v>
       </c>
+      <c r="C41" t="s">
+        <v>42</v>
+      </c>
+      <c r="D41" t="s">
+        <v>42</v>
+      </c>
+      <c r="E41" t="s">
+        <v>42</v>
+      </c>
       <c r="F41" t="s">
         <v>21</v>
       </c>
@@ -1373,6 +1743,15 @@
       <c r="B42" t="s">
         <v>10</v>
       </c>
+      <c r="C42" t="s">
+        <v>42</v>
+      </c>
+      <c r="D42" t="s">
+        <v>42</v>
+      </c>
+      <c r="E42" t="s">
+        <v>42</v>
+      </c>
       <c r="F42" t="s">
         <v>40</v>
       </c>
@@ -1387,6 +1766,15 @@
       <c r="B43" t="s">
         <v>10</v>
       </c>
+      <c r="C43" t="s">
+        <v>42</v>
+      </c>
+      <c r="D43" t="s">
+        <v>42</v>
+      </c>
+      <c r="E43" t="s">
+        <v>42</v>
+      </c>
       <c r="F43" t="s">
         <v>25</v>
       </c>
@@ -1395,6 +1783,11 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:G43">
+    <sortState ref="A2:G43">
+      <sortCondition ref="A1:A43"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add A/B m7 chords
</commit_message>
<xml_diff>
--- a/Chord_Chart_Source.xlsx
+++ b/Chord_Chart_Source.xlsx
@@ -16,7 +16,7 @@
     <sheet name="Chords" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Chords!$A$1:$D$67</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Chords!$A$1:$D$75</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="41">
   <si>
     <t>Note</t>
   </si>
@@ -148,6 +148,9 @@
   </si>
   <si>
     <t>1B</t>
+  </si>
+  <si>
+    <t>m7</t>
   </si>
 </sst>
 </file>
@@ -769,10 +772,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D71"/>
+  <dimension ref="A1:D79"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -936,13 +939,13 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>6</v>
+        <v>40</v>
       </c>
       <c r="C12" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -950,44 +953,44 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B13" t="s">
-        <v>6</v>
+        <v>40</v>
       </c>
       <c r="C13" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="D13">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B14" t="s">
-        <v>6</v>
+        <v>40</v>
       </c>
       <c r="C14" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="D14">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B15" t="s">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="C15" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="D15">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
@@ -995,13 +998,13 @@
         <v>10</v>
       </c>
       <c r="B16" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C16" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="D16">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
@@ -1009,52 +1012,52 @@
         <v>10</v>
       </c>
       <c r="B17" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D17">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>10</v>
       </c>
-      <c r="B18">
-        <v>7</v>
+      <c r="B18" t="s">
+        <v>6</v>
       </c>
       <c r="C18" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D18">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>10</v>
       </c>
-      <c r="B19">
-        <v>7</v>
+      <c r="B19" t="s">
+        <v>8</v>
       </c>
       <c r="C19" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="D19">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>10</v>
       </c>
-      <c r="B20">
-        <v>7</v>
+      <c r="B20" t="s">
+        <v>8</v>
       </c>
       <c r="C20" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="D20">
         <v>3</v>
@@ -1064,11 +1067,11 @@
       <c r="A21" t="s">
         <v>10</v>
       </c>
-      <c r="B21">
-        <v>7</v>
+      <c r="B21" t="s">
+        <v>8</v>
       </c>
       <c r="C21" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="D21">
         <v>5</v>
@@ -1076,13 +1079,13 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>4</v>
-      </c>
-      <c r="B22" t="s">
-        <v>6</v>
+        <v>10</v>
+      </c>
+      <c r="B22">
+        <v>7</v>
       </c>
       <c r="C22" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="D22">
         <v>1</v>
@@ -1090,692 +1093,804 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>4</v>
-      </c>
-      <c r="B23" t="s">
-        <v>6</v>
+        <v>10</v>
+      </c>
+      <c r="B23">
+        <v>7</v>
       </c>
       <c r="C23" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="D23">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>4</v>
-      </c>
-      <c r="B24" t="s">
-        <v>6</v>
+        <v>10</v>
+      </c>
+      <c r="B24">
+        <v>7</v>
       </c>
       <c r="C24" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="D24">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>4</v>
-      </c>
-      <c r="B25" t="s">
-        <v>8</v>
+        <v>10</v>
+      </c>
+      <c r="B25">
+        <v>7</v>
       </c>
       <c r="C25" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D25">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B26" t="s">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="C26" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="D26">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B27" t="s">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="C27" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="D27">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>4</v>
-      </c>
-      <c r="B28">
-        <v>7</v>
+        <v>10</v>
+      </c>
+      <c r="B28" t="s">
+        <v>40</v>
       </c>
       <c r="C28" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="D28">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>4</v>
-      </c>
-      <c r="B29">
-        <v>7</v>
+        <v>10</v>
+      </c>
+      <c r="B29" t="s">
+        <v>40</v>
       </c>
       <c r="C29" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D29">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>4</v>
       </c>
-      <c r="B30">
-        <v>7</v>
+      <c r="B30" t="s">
+        <v>6</v>
       </c>
       <c r="C30" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D30">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>4</v>
       </c>
-      <c r="B31">
-        <v>7</v>
+      <c r="B31" t="s">
+        <v>6</v>
       </c>
       <c r="C31" t="s">
-        <v>38</v>
+        <v>17</v>
       </c>
       <c r="D31">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="B32" t="s">
         <v>6</v>
       </c>
       <c r="C32" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D32">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="B33" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C33" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="D33">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="B34" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C34" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="D34">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="B35" t="s">
         <v>8</v>
       </c>
       <c r="C35" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D35">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>11</v>
-      </c>
-      <c r="B36" t="s">
-        <v>8</v>
+        <v>4</v>
+      </c>
+      <c r="B36">
+        <v>7</v>
       </c>
       <c r="C36" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D36">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>11</v>
-      </c>
-      <c r="B37" t="s">
-        <v>8</v>
+        <v>4</v>
+      </c>
+      <c r="B37">
+        <v>7</v>
       </c>
       <c r="C37" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
       <c r="D37">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="B38">
         <v>7</v>
       </c>
       <c r="C38" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D38">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="B39">
         <v>7</v>
       </c>
       <c r="C39" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="D39">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>11</v>
       </c>
-      <c r="B40">
-        <v>7</v>
+      <c r="B40" t="s">
+        <v>6</v>
       </c>
       <c r="C40" t="s">
-        <v>37</v>
+        <v>16</v>
       </c>
       <c r="D40">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>11</v>
       </c>
-      <c r="B41">
-        <v>7</v>
+      <c r="B41" t="s">
+        <v>6</v>
       </c>
       <c r="C41" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="D41">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B42" t="s">
         <v>6</v>
       </c>
       <c r="C42" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="D42">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B43" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C43" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="D43">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B44" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C44" t="s">
-        <v>39</v>
+        <v>18</v>
       </c>
       <c r="D44">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B45" t="s">
         <v>8</v>
       </c>
       <c r="C45" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="D45">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>12</v>
-      </c>
-      <c r="B46" t="s">
-        <v>8</v>
+        <v>11</v>
+      </c>
+      <c r="B46">
+        <v>7</v>
       </c>
       <c r="C46" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D46">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>12</v>
-      </c>
-      <c r="B47" t="s">
-        <v>8</v>
+        <v>11</v>
+      </c>
+      <c r="B47">
+        <v>7</v>
       </c>
       <c r="C47" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="D47">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B48">
         <v>7</v>
       </c>
       <c r="C48" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="D48">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B49">
         <v>7</v>
       </c>
       <c r="C49" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="D49">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>12</v>
       </c>
-      <c r="B50">
-        <v>7</v>
+      <c r="B50" t="s">
+        <v>6</v>
       </c>
       <c r="C50" t="s">
-        <v>39</v>
+        <v>17</v>
       </c>
       <c r="D50">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>12</v>
       </c>
-      <c r="B51">
-        <v>7</v>
+      <c r="B51" t="s">
+        <v>6</v>
       </c>
       <c r="C51" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D51">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B52" t="s">
         <v>6</v>
       </c>
       <c r="C52" t="s">
-        <v>18</v>
+        <v>39</v>
       </c>
       <c r="D52">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B53" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C53" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
       <c r="D53">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B54" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C54" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D54">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B55" t="s">
         <v>8</v>
       </c>
       <c r="C55" t="s">
-        <v>18</v>
+        <v>39</v>
       </c>
       <c r="D55">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>13</v>
-      </c>
-      <c r="B56" t="s">
-        <v>8</v>
+        <v>12</v>
+      </c>
+      <c r="B56">
+        <v>7</v>
       </c>
       <c r="C56" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="D56">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>13</v>
-      </c>
-      <c r="B57" t="s">
-        <v>8</v>
+        <v>12</v>
+      </c>
+      <c r="B57">
+        <v>7</v>
       </c>
       <c r="C57" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="D57">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B58">
         <v>7</v>
       </c>
       <c r="C58" t="s">
-        <v>18</v>
+        <v>39</v>
       </c>
       <c r="D58">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B59">
         <v>7</v>
       </c>
       <c r="C59" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="D59">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>13</v>
       </c>
-      <c r="B60">
-        <v>7</v>
+      <c r="B60" t="s">
+        <v>6</v>
       </c>
       <c r="C60" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D60">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>13</v>
       </c>
-      <c r="B61">
-        <v>7</v>
+      <c r="B61" t="s">
+        <v>6</v>
       </c>
       <c r="C61" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="D61">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B62" t="s">
         <v>6</v>
       </c>
       <c r="C62" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D62">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B63" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C63" t="s">
-        <v>39</v>
+        <v>18</v>
       </c>
       <c r="D63">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B64" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C64" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D64">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B65" t="s">
         <v>8</v>
       </c>
       <c r="C65" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D65">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>14</v>
-      </c>
-      <c r="B66" t="s">
-        <v>8</v>
+        <v>13</v>
+      </c>
+      <c r="B66">
+        <v>7</v>
       </c>
       <c r="C66" t="s">
-        <v>38</v>
+        <v>18</v>
       </c>
       <c r="D66">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>14</v>
-      </c>
-      <c r="B67" t="s">
-        <v>8</v>
+        <v>13</v>
+      </c>
+      <c r="B67">
+        <v>7</v>
       </c>
       <c r="C67" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="D67">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B68">
         <v>7</v>
       </c>
       <c r="C68" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D68">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B69">
         <v>7</v>
       </c>
       <c r="C69" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="D69">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>14</v>
       </c>
-      <c r="B70">
-        <v>7</v>
+      <c r="B70" t="s">
+        <v>6</v>
       </c>
       <c r="C70" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D70">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>14</v>
       </c>
-      <c r="B71">
-        <v>7</v>
+      <c r="B71" t="s">
+        <v>6</v>
       </c>
       <c r="C71" t="s">
+        <v>39</v>
+      </c>
+      <c r="D71">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>14</v>
+      </c>
+      <c r="B72" t="s">
+        <v>6</v>
+      </c>
+      <c r="C72" t="s">
+        <v>23</v>
+      </c>
+      <c r="D72">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>14</v>
+      </c>
+      <c r="B73" t="s">
+        <v>8</v>
+      </c>
+      <c r="C73" t="s">
+        <v>19</v>
+      </c>
+      <c r="D73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>14</v>
+      </c>
+      <c r="B74" t="s">
+        <v>8</v>
+      </c>
+      <c r="C74" t="s">
+        <v>38</v>
+      </c>
+      <c r="D74">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>14</v>
+      </c>
+      <c r="B75" t="s">
+        <v>8</v>
+      </c>
+      <c r="C75" t="s">
+        <v>23</v>
+      </c>
+      <c r="D75">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>14</v>
+      </c>
+      <c r="B76">
+        <v>7</v>
+      </c>
+      <c r="C76" t="s">
+        <v>19</v>
+      </c>
+      <c r="D76">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>14</v>
+      </c>
+      <c r="B77">
+        <v>7</v>
+      </c>
+      <c r="C77" t="s">
+        <v>39</v>
+      </c>
+      <c r="D77">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>14</v>
+      </c>
+      <c r="B78">
+        <v>7</v>
+      </c>
+      <c r="C78" t="s">
+        <v>23</v>
+      </c>
+      <c r="D78">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>14</v>
+      </c>
+      <c r="B79">
+        <v>7</v>
+      </c>
+      <c r="C79" t="s">
         <v>25</v>
       </c>
-      <c r="D71">
+      <c r="D79">
         <v>5</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D67">
+  <autoFilter ref="A1:D75">
     <sortState ref="A2:G43">
       <sortCondition ref="A1:A43"/>
     </sortState>

</xml_diff>

<commit_message>
Add Remaining m7 chords
Updated extract
</commit_message>
<xml_diff>
--- a/Chord_Chart_Source.xlsx
+++ b/Chord_Chart_Source.xlsx
@@ -9,14 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15480" windowHeight="7452"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15480" windowHeight="7452" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Basic Notes" sheetId="1" r:id="rId1"/>
     <sheet name="Chords" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Chords!$A$1:$D$75</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Chords!$A$1:$D$91</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="41">
   <si>
     <t>Note</t>
   </si>
@@ -470,7 +470,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
@@ -772,10 +772,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D79"/>
+  <dimension ref="A1:D99"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
+      <selection activeCell="A99" sqref="A99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1331,13 +1331,13 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="B40" t="s">
-        <v>6</v>
+        <v>40</v>
       </c>
       <c r="C40" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D40">
         <v>1</v>
@@ -1345,44 +1345,44 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="B41" t="s">
-        <v>6</v>
+        <v>40</v>
       </c>
       <c r="C41" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D41">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="B42" t="s">
-        <v>6</v>
+        <v>40</v>
       </c>
       <c r="C42" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="D42">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="B43" t="s">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="C43" t="s">
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="D43">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
@@ -1390,13 +1390,13 @@
         <v>11</v>
       </c>
       <c r="B44" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C44" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D44">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
@@ -1404,52 +1404,52 @@
         <v>11</v>
       </c>
       <c r="B45" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C45" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="D45">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>11</v>
       </c>
-      <c r="B46">
-        <v>7</v>
+      <c r="B46" t="s">
+        <v>6</v>
       </c>
       <c r="C46" t="s">
-        <v>16</v>
+        <v>37</v>
       </c>
       <c r="D46">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>11</v>
       </c>
-      <c r="B47">
-        <v>7</v>
+      <c r="B47" t="s">
+        <v>8</v>
       </c>
       <c r="C47" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="D47">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>11</v>
       </c>
-      <c r="B48">
-        <v>7</v>
+      <c r="B48" t="s">
+        <v>8</v>
       </c>
       <c r="C48" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="D48">
         <v>3</v>
@@ -1459,11 +1459,11 @@
       <c r="A49" t="s">
         <v>11</v>
       </c>
-      <c r="B49">
-        <v>7</v>
+      <c r="B49" t="s">
+        <v>8</v>
       </c>
       <c r="C49" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="D49">
         <v>5</v>
@@ -1471,13 +1471,13 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>12</v>
-      </c>
-      <c r="B50" t="s">
-        <v>6</v>
+        <v>11</v>
+      </c>
+      <c r="B50">
+        <v>7</v>
       </c>
       <c r="C50" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D50">
         <v>1</v>
@@ -1485,412 +1485,692 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>12</v>
-      </c>
-      <c r="B51" t="s">
-        <v>6</v>
+        <v>11</v>
+      </c>
+      <c r="B51">
+        <v>7</v>
       </c>
       <c r="C51" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D51">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>12</v>
-      </c>
-      <c r="B52" t="s">
-        <v>6</v>
+        <v>11</v>
+      </c>
+      <c r="B52">
+        <v>7</v>
       </c>
       <c r="C52" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D52">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>12</v>
-      </c>
-      <c r="B53" t="s">
-        <v>8</v>
+        <v>11</v>
+      </c>
+      <c r="B53">
+        <v>7</v>
       </c>
       <c r="C53" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="D53">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B54" t="s">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="C54" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D54">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B55" t="s">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="C55" t="s">
-        <v>39</v>
+        <v>18</v>
       </c>
       <c r="D55">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>12</v>
-      </c>
-      <c r="B56">
-        <v>7</v>
+        <v>11</v>
+      </c>
+      <c r="B56" t="s">
+        <v>40</v>
       </c>
       <c r="C56" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="D56">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>12</v>
-      </c>
-      <c r="B57">
-        <v>7</v>
+        <v>11</v>
+      </c>
+      <c r="B57" t="s">
+        <v>40</v>
       </c>
       <c r="C57" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="D57">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>12</v>
       </c>
-      <c r="B58">
-        <v>7</v>
+      <c r="B58" t="s">
+        <v>6</v>
       </c>
       <c r="C58" t="s">
-        <v>39</v>
+        <v>17</v>
       </c>
       <c r="D58">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>12</v>
       </c>
-      <c r="B59">
-        <v>7</v>
+      <c r="B59" t="s">
+        <v>6</v>
       </c>
       <c r="C59" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D59">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B60" t="s">
         <v>6</v>
       </c>
       <c r="C60" t="s">
-        <v>18</v>
+        <v>39</v>
       </c>
       <c r="D60">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B61" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C61" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
       <c r="D61">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B62" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C62" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D62">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B63" t="s">
         <v>8</v>
       </c>
       <c r="C63" t="s">
-        <v>18</v>
+        <v>39</v>
       </c>
       <c r="D63">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>13</v>
-      </c>
-      <c r="B64" t="s">
-        <v>8</v>
+        <v>12</v>
+      </c>
+      <c r="B64">
+        <v>7</v>
       </c>
       <c r="C64" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="D64">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>13</v>
-      </c>
-      <c r="B65" t="s">
-        <v>8</v>
+        <v>12</v>
+      </c>
+      <c r="B65">
+        <v>7</v>
       </c>
       <c r="C65" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="D65">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B66">
         <v>7</v>
       </c>
       <c r="C66" t="s">
-        <v>18</v>
+        <v>39</v>
       </c>
       <c r="D66">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B67">
         <v>7</v>
       </c>
       <c r="C67" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="D67">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>13</v>
-      </c>
-      <c r="B68">
-        <v>7</v>
+        <v>12</v>
+      </c>
+      <c r="B68" t="s">
+        <v>40</v>
       </c>
       <c r="C68" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D68">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>13</v>
-      </c>
-      <c r="B69">
-        <v>7</v>
+        <v>12</v>
+      </c>
+      <c r="B69" t="s">
+        <v>40</v>
       </c>
       <c r="C69" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="D69">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B70" t="s">
-        <v>6</v>
+        <v>40</v>
       </c>
       <c r="C70" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="D70">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B71" t="s">
-        <v>6</v>
+        <v>40</v>
       </c>
       <c r="C71" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="D71">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B72" t="s">
         <v>6</v>
       </c>
       <c r="C72" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="D72">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B73" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C73" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="D73">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B74" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C74" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="D74">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B75" t="s">
         <v>8</v>
       </c>
       <c r="C75" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="D75">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>14</v>
-      </c>
-      <c r="B76">
-        <v>7</v>
+        <v>13</v>
+      </c>
+      <c r="B76" t="s">
+        <v>8</v>
       </c>
       <c r="C76" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="D76">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>14</v>
-      </c>
-      <c r="B77">
-        <v>7</v>
+        <v>13</v>
+      </c>
+      <c r="B77" t="s">
+        <v>8</v>
       </c>
       <c r="C77" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
       <c r="D77">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B78">
         <v>7</v>
       </c>
       <c r="C78" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="D78">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
+        <v>13</v>
+      </c>
+      <c r="B79">
+        <v>7</v>
+      </c>
+      <c r="C79" t="s">
+        <v>37</v>
+      </c>
+      <c r="D79">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>13</v>
+      </c>
+      <c r="B80">
+        <v>7</v>
+      </c>
+      <c r="C80" t="s">
+        <v>22</v>
+      </c>
+      <c r="D80">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>13</v>
+      </c>
+      <c r="B81">
+        <v>7</v>
+      </c>
+      <c r="C81" t="s">
+        <v>34</v>
+      </c>
+      <c r="D81">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>13</v>
+      </c>
+      <c r="B82" t="s">
+        <v>40</v>
+      </c>
+      <c r="C82" t="s">
+        <v>18</v>
+      </c>
+      <c r="D82">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>13</v>
+      </c>
+      <c r="B83" t="s">
+        <v>40</v>
+      </c>
+      <c r="C83" t="s">
+        <v>31</v>
+      </c>
+      <c r="D83">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>13</v>
+      </c>
+      <c r="B84" t="s">
+        <v>40</v>
+      </c>
+      <c r="C84" t="s">
+        <v>22</v>
+      </c>
+      <c r="D84">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>13</v>
+      </c>
+      <c r="B85" t="s">
+        <v>40</v>
+      </c>
+      <c r="C85" t="s">
+        <v>34</v>
+      </c>
+      <c r="D85">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
         <v>14</v>
       </c>
-      <c r="B79">
-        <v>7</v>
-      </c>
-      <c r="C79" t="s">
+      <c r="B86" t="s">
+        <v>6</v>
+      </c>
+      <c r="C86" t="s">
+        <v>19</v>
+      </c>
+      <c r="D86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
+        <v>14</v>
+      </c>
+      <c r="B87" t="s">
+        <v>6</v>
+      </c>
+      <c r="C87" t="s">
+        <v>39</v>
+      </c>
+      <c r="D87">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>14</v>
+      </c>
+      <c r="B88" t="s">
+        <v>6</v>
+      </c>
+      <c r="C88" t="s">
+        <v>23</v>
+      </c>
+      <c r="D88">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
+        <v>14</v>
+      </c>
+      <c r="B89" t="s">
+        <v>8</v>
+      </c>
+      <c r="C89" t="s">
+        <v>19</v>
+      </c>
+      <c r="D89">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
+        <v>14</v>
+      </c>
+      <c r="B90" t="s">
+        <v>8</v>
+      </c>
+      <c r="C90" t="s">
+        <v>38</v>
+      </c>
+      <c r="D90">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
+        <v>14</v>
+      </c>
+      <c r="B91" t="s">
+        <v>8</v>
+      </c>
+      <c r="C91" t="s">
+        <v>23</v>
+      </c>
+      <c r="D91">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
+        <v>14</v>
+      </c>
+      <c r="B92">
+        <v>7</v>
+      </c>
+      <c r="C92" t="s">
+        <v>19</v>
+      </c>
+      <c r="D92">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
+        <v>14</v>
+      </c>
+      <c r="B93">
+        <v>7</v>
+      </c>
+      <c r="C93" t="s">
+        <v>39</v>
+      </c>
+      <c r="D93">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
+        <v>14</v>
+      </c>
+      <c r="B94">
+        <v>7</v>
+      </c>
+      <c r="C94" t="s">
+        <v>23</v>
+      </c>
+      <c r="D94">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
+        <v>14</v>
+      </c>
+      <c r="B95">
+        <v>7</v>
+      </c>
+      <c r="C95" t="s">
         <v>25</v>
       </c>
-      <c r="D79">
+      <c r="D95">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
+        <v>14</v>
+      </c>
+      <c r="B96" t="s">
+        <v>40</v>
+      </c>
+      <c r="C96" t="s">
+        <v>19</v>
+      </c>
+      <c r="D96">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
+        <v>14</v>
+      </c>
+      <c r="B97" t="s">
+        <v>40</v>
+      </c>
+      <c r="C97" t="s">
+        <v>38</v>
+      </c>
+      <c r="D97">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
+        <v>14</v>
+      </c>
+      <c r="B98" t="s">
+        <v>40</v>
+      </c>
+      <c r="C98" t="s">
+        <v>23</v>
+      </c>
+      <c r="D98">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
+        <v>14</v>
+      </c>
+      <c r="B99" t="s">
+        <v>40</v>
+      </c>
+      <c r="C99" t="s">
+        <v>25</v>
+      </c>
+      <c r="D99">
         <v>5</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D75">
+  <autoFilter ref="A1:D91">
     <sortState ref="A2:G43">
       <sortCondition ref="A1:A43"/>
     </sortState>

</xml_diff>